<commit_message>
Product and User services
</commit_message>
<xml_diff>
--- a/backendHappyPockets/src/main/java/com/happyPockets/service/productos.xlsx
+++ b/backendHappyPockets/src/main/java/com/happyPockets/service/productos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Dev-offline\iis\backendHappyPockets\src\main\java\com\happyPockets\service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\proyecto-IS\backendHappyPockets\src\main\java\com\happyPockets\service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE278DD6-CF85-4EE9-A57B-97F1774CCA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F15FD21-F0AF-478E-AF76-D96446B12DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{F1208974-05B8-4F0C-80C5-DBE5275A8570}"/>
+    <workbookView xWindow="3996" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{F1208974-05B8-4F0C-80C5-DBE5275A8570}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -519,6 +519,20 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
@@ -551,20 +565,6 @@
         <right/>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -617,10 +617,10 @@
     <tableColumn id="1" xr3:uid="{D78518C3-3267-4FA3-B1EA-CEE9C58C6F66}" name="Nombre" dataDxfId="5"/>
     <tableColumn id="9" xr3:uid="{E3C577AD-005A-48A9-B8F2-191D3A2D090B}" name="Marca"/>
     <tableColumn id="2" xr3:uid="{09ADEF9E-55BE-4D2D-832F-30BC0E58734B}" name="Categoria" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{EB603D68-57B0-440B-96E6-4E6D72C48070}" name="Precio" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{277071FF-019C-46E7-9582-1010EA734DDD}" name="Precio2" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{600208F2-9E7D-46C4-8493-054015362597}" name="Precio4" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{BAC4EC4E-C8C1-4253-BEBC-DACA7322471F}" name="Imagen(url)3" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{EB603D68-57B0-440B-96E6-4E6D72C48070}" name="Precio" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{277071FF-019C-46E7-9582-1010EA734DDD}" name="Precio2" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{600208F2-9E7D-46C4-8493-054015362597}" name="Precio4" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{BAC4EC4E-C8C1-4253-BEBC-DACA7322471F}" name="Imagen(url)3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -949,17 +949,17 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.1328125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.53125" customWidth="1"/>
-    <col min="3" max="3" width="20.1328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.53125" style="14" customWidth="1"/>
-    <col min="5" max="6" width="13.53125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="86.1328125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="14" customWidth="1"/>
+    <col min="5" max="6" width="13.5546875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="86.109375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="8"/>
       <c r="C1" s="7"/>
@@ -974,7 +974,7 @@
       </c>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -997,7 +997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>61</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>84</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>73</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>80</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>68</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>65</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>39</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>54</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>59</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>78</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>88</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>14</v>
       </c>
@@ -1503,931 +1503,931 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F25" s="19"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F26" s="19"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F27" s="19"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F28" s="19"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F29" s="19"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F30" s="19"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F31" s="19"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F32" s="19"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F33" s="19"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F34" s="19"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F35" s="19"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F36" s="19"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F37" s="19"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F38" s="19"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F39" s="19"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F40" s="19"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F41" s="19"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F42" s="19"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F43" s="19"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F44" s="19"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F45" s="19"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F46" s="19"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F47" s="19"/>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F48" s="19"/>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F49" s="19"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F50" s="19"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F51" s="19"/>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F52" s="19"/>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F53" s="19"/>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F54" s="19"/>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F55" s="19"/>
       <c r="G55" s="5"/>
     </row>
-    <row r="56" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F56" s="19"/>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F57" s="19"/>
       <c r="G57" s="5"/>
     </row>
-    <row r="58" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F58" s="19"/>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F59" s="19"/>
       <c r="G59" s="5"/>
     </row>
-    <row r="60" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F60" s="19"/>
       <c r="G60" s="5"/>
     </row>
-    <row r="61" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F61" s="19"/>
       <c r="G61" s="5"/>
     </row>
-    <row r="62" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F62" s="19"/>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F63" s="19"/>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F64" s="19"/>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F65" s="19"/>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F66" s="19"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F67" s="19"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F68" s="19"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F69" s="19"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F70" s="19"/>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F71" s="19"/>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F72" s="19"/>
       <c r="G72" s="5"/>
     </row>
-    <row r="73" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F73" s="19"/>
       <c r="G73" s="5"/>
     </row>
-    <row r="74" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F74" s="19"/>
       <c r="G74" s="5"/>
     </row>
-    <row r="75" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F75" s="19"/>
       <c r="G75" s="5"/>
     </row>
-    <row r="76" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F76" s="19"/>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="77" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F77" s="19"/>
       <c r="G77" s="5"/>
     </row>
-    <row r="78" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="78" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F78" s="19"/>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="79" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F79" s="19"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="80" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F80" s="19"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F81" s="19"/>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F82" s="19"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F83" s="19"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F84" s="19"/>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F85" s="19"/>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F86" s="19"/>
       <c r="G86" s="5"/>
     </row>
-    <row r="87" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F87" s="19"/>
       <c r="G87" s="5"/>
     </row>
-    <row r="88" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F88" s="19"/>
       <c r="G88" s="5"/>
     </row>
-    <row r="89" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F89" s="19"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F90" s="19"/>
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F91" s="19"/>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F92" s="19"/>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F93" s="19"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F94" s="19"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F95" s="19"/>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F96" s="19"/>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F97" s="19"/>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F98" s="19"/>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F99" s="19"/>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="100" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F100" s="19"/>
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="101" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F101" s="19"/>
       <c r="G101" s="5"/>
     </row>
-    <row r="102" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="102" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F102" s="19"/>
       <c r="G102" s="5"/>
     </row>
-    <row r="103" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="103" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F103" s="19"/>
       <c r="G103" s="5"/>
     </row>
-    <row r="104" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="104" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F104" s="19"/>
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F105" s="19"/>
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="106" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F106" s="19"/>
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="107" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F107" s="19"/>
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="108" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F108" s="19"/>
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="109" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F109" s="19"/>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="110" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F110" s="19"/>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="111" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F111" s="19"/>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="112" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F112" s="19"/>
       <c r="G112" s="5"/>
     </row>
-    <row r="113" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="113" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F113" s="19"/>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="114" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F114" s="19"/>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="115" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F115" s="19"/>
       <c r="G115" s="5"/>
     </row>
-    <row r="116" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="116" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F116" s="19"/>
       <c r="G116" s="5"/>
     </row>
-    <row r="117" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="117" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F117" s="19"/>
       <c r="G117" s="5"/>
     </row>
-    <row r="118" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="118" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F118" s="19"/>
       <c r="G118" s="5"/>
     </row>
-    <row r="119" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="119" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F119" s="19"/>
       <c r="G119" s="5"/>
     </row>
-    <row r="120" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="120" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F120" s="19"/>
       <c r="G120" s="5"/>
     </row>
-    <row r="121" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="121" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F121" s="19"/>
       <c r="G121" s="5"/>
     </row>
-    <row r="122" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="122" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F122" s="19"/>
       <c r="G122" s="5"/>
     </row>
-    <row r="123" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="123" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F123" s="19"/>
       <c r="G123" s="5"/>
     </row>
-    <row r="124" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="124" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F124" s="19"/>
       <c r="G124" s="5"/>
     </row>
-    <row r="125" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="125" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F125" s="19"/>
       <c r="G125" s="5"/>
     </row>
-    <row r="126" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="126" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F126" s="19"/>
       <c r="G126" s="5"/>
     </row>
-    <row r="127" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="127" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F127" s="19"/>
       <c r="G127" s="5"/>
     </row>
-    <row r="128" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="128" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F128" s="19"/>
       <c r="G128" s="5"/>
     </row>
-    <row r="129" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="129" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F129" s="19"/>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="130" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F130" s="19"/>
       <c r="G130" s="5"/>
     </row>
-    <row r="131" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="131" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F131" s="19"/>
       <c r="G131" s="5"/>
     </row>
-    <row r="132" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="132" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F132" s="19"/>
       <c r="G132" s="5"/>
     </row>
-    <row r="133" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="133" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F133" s="19"/>
       <c r="G133" s="5"/>
     </row>
-    <row r="134" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="134" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F134" s="19"/>
       <c r="G134" s="5"/>
     </row>
-    <row r="135" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="135" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F135" s="19"/>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="136" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F136" s="19"/>
       <c r="G136" s="5"/>
     </row>
-    <row r="137" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="137" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F137" s="19"/>
       <c r="G137" s="5"/>
     </row>
-    <row r="138" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="138" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F138" s="19"/>
       <c r="G138" s="5"/>
     </row>
-    <row r="139" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="139" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F139" s="19"/>
       <c r="G139" s="5"/>
     </row>
-    <row r="140" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="140" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F140" s="19"/>
       <c r="G140" s="5"/>
     </row>
-    <row r="141" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="141" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F141" s="19"/>
       <c r="G141" s="5"/>
     </row>
-    <row r="142" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="142" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F142" s="19"/>
       <c r="G142" s="5"/>
     </row>
-    <row r="143" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="143" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F143" s="19"/>
       <c r="G143" s="5"/>
     </row>
-    <row r="144" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="144" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F144" s="19"/>
       <c r="G144" s="5"/>
     </row>
-    <row r="145" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="145" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F145" s="19"/>
       <c r="G145" s="5"/>
     </row>
-    <row r="146" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="146" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F146" s="19"/>
       <c r="G146" s="5"/>
     </row>
-    <row r="147" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="147" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F147" s="19"/>
       <c r="G147" s="5"/>
     </row>
-    <row r="148" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="148" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F148" s="19"/>
       <c r="G148" s="5"/>
     </row>
-    <row r="149" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="149" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F149" s="19"/>
       <c r="G149" s="5"/>
     </row>
-    <row r="150" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="150" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F150" s="19"/>
       <c r="G150" s="5"/>
     </row>
-    <row r="151" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="151" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F151" s="19"/>
       <c r="G151" s="5"/>
     </row>
-    <row r="152" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="152" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F152" s="19"/>
       <c r="G152" s="5"/>
     </row>
-    <row r="153" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="153" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F153" s="19"/>
       <c r="G153" s="5"/>
     </row>
-    <row r="154" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="154" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F154" s="19"/>
       <c r="G154" s="5"/>
     </row>
-    <row r="155" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="155" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F155" s="19"/>
       <c r="G155" s="5"/>
     </row>
-    <row r="156" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="156" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F156" s="19"/>
       <c r="G156" s="5"/>
     </row>
-    <row r="157" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="157" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F157" s="19"/>
       <c r="G157" s="5"/>
     </row>
-    <row r="158" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="158" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F158" s="19"/>
       <c r="G158" s="5"/>
     </row>
-    <row r="159" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="159" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F159" s="19"/>
       <c r="G159" s="5"/>
     </row>
-    <row r="160" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="160" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F160" s="19"/>
       <c r="G160" s="5"/>
     </row>
-    <row r="161" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="161" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F161" s="19"/>
       <c r="G161" s="5"/>
     </row>
-    <row r="162" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="162" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F162" s="19"/>
       <c r="G162" s="5"/>
     </row>
-    <row r="163" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="163" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F163" s="19"/>
       <c r="G163" s="5"/>
     </row>
-    <row r="164" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="164" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F164" s="19"/>
       <c r="G164" s="5"/>
     </row>
-    <row r="165" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="165" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F165" s="19"/>
       <c r="G165" s="5"/>
     </row>
-    <row r="166" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="166" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F166" s="19"/>
       <c r="G166" s="5"/>
     </row>
-    <row r="167" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="167" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F167" s="19"/>
       <c r="G167" s="5"/>
     </row>
-    <row r="168" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="168" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F168" s="19"/>
       <c r="G168" s="5"/>
     </row>
-    <row r="169" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="169" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F169" s="19"/>
       <c r="G169" s="5"/>
     </row>
-    <row r="170" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="170" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F170" s="19"/>
       <c r="G170" s="5"/>
     </row>
-    <row r="171" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="171" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F171" s="19"/>
       <c r="G171" s="5"/>
     </row>
-    <row r="172" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="172" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F172" s="19"/>
       <c r="G172" s="5"/>
     </row>
-    <row r="173" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="173" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F173" s="19"/>
       <c r="G173" s="5"/>
     </row>
-    <row r="174" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="174" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F174" s="19"/>
       <c r="G174" s="5"/>
     </row>
-    <row r="175" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="175" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F175" s="19"/>
       <c r="G175" s="5"/>
     </row>
-    <row r="176" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="176" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F176" s="19"/>
       <c r="G176" s="5"/>
     </row>
-    <row r="177" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="177" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F177" s="19"/>
       <c r="G177" s="5"/>
     </row>
-    <row r="178" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="178" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F178" s="19"/>
       <c r="G178" s="5"/>
     </row>
-    <row r="179" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="179" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F179" s="19"/>
       <c r="G179" s="5"/>
     </row>
-    <row r="180" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="180" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F180" s="19"/>
       <c r="G180" s="5"/>
     </row>
-    <row r="181" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="181" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F181" s="19"/>
       <c r="G181" s="5"/>
     </row>
-    <row r="182" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="182" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F182" s="19"/>
       <c r="G182" s="5"/>
     </row>
-    <row r="183" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="183" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F183" s="19"/>
       <c r="G183" s="5"/>
     </row>
-    <row r="184" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="184" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F184" s="19"/>
       <c r="G184" s="5"/>
     </row>
-    <row r="185" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="185" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F185" s="19"/>
       <c r="G185" s="5"/>
     </row>
-    <row r="186" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="186" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F186" s="19"/>
       <c r="G186" s="5"/>
     </row>
-    <row r="187" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="187" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F187" s="19"/>
       <c r="G187" s="5"/>
     </row>
-    <row r="188" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="188" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F188" s="19"/>
       <c r="G188" s="5"/>
     </row>
-    <row r="189" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="189" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F189" s="19"/>
       <c r="G189" s="5"/>
     </row>
-    <row r="190" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="190" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F190" s="19"/>
       <c r="G190" s="5"/>
     </row>
-    <row r="191" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="191" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F191" s="19"/>
       <c r="G191" s="5"/>
     </row>
-    <row r="192" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="192" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F192" s="19"/>
       <c r="G192" s="5"/>
     </row>
-    <row r="193" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="193" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F193" s="19"/>
       <c r="G193" s="5"/>
     </row>
-    <row r="194" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="194" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F194" s="19"/>
       <c r="G194" s="5"/>
     </row>
-    <row r="195" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="195" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F195" s="19"/>
       <c r="G195" s="5"/>
     </row>
-    <row r="196" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="196" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F196" s="19"/>
       <c r="G196" s="5"/>
     </row>
-    <row r="197" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="197" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F197" s="19"/>
       <c r="G197" s="5"/>
     </row>
-    <row r="198" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="198" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F198" s="19"/>
       <c r="G198" s="5"/>
     </row>
-    <row r="199" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="199" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F199" s="19"/>
       <c r="G199" s="5"/>
     </row>
-    <row r="200" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="200" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F200" s="19"/>
       <c r="G200" s="5"/>
     </row>
-    <row r="201" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="201" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F201" s="19"/>
       <c r="G201" s="5"/>
     </row>
-    <row r="202" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="202" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F202" s="19"/>
       <c r="G202" s="5"/>
     </row>
-    <row r="203" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="203" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F203" s="19"/>
       <c r="G203" s="5"/>
     </row>
-    <row r="204" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="204" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F204" s="19"/>
       <c r="G204" s="5"/>
     </row>
-    <row r="205" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="205" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F205" s="19"/>
       <c r="G205" s="5"/>
     </row>
-    <row r="206" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="206" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F206" s="19"/>
       <c r="G206" s="5"/>
     </row>
-    <row r="207" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="207" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F207" s="19"/>
       <c r="G207" s="5"/>
     </row>
-    <row r="208" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="208" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F208" s="19"/>
       <c r="G208" s="5"/>
     </row>
-    <row r="209" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="209" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F209" s="19"/>
       <c r="G209" s="5"/>
     </row>
-    <row r="210" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="210" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F210" s="19"/>
       <c r="G210" s="5"/>
     </row>
-    <row r="211" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="211" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F211" s="19"/>
       <c r="G211" s="5"/>
     </row>
-    <row r="212" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="212" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F212" s="19"/>
       <c r="G212" s="5"/>
     </row>
-    <row r="213" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="213" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F213" s="19"/>
       <c r="G213" s="5"/>
     </row>
-    <row r="214" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="214" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F214" s="19"/>
       <c r="G214" s="5"/>
     </row>
-    <row r="215" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="215" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F215" s="19"/>
       <c r="G215" s="5"/>
     </row>
-    <row r="216" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="216" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F216" s="19"/>
       <c r="G216" s="5"/>
     </row>
-    <row r="217" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="217" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F217" s="19"/>
       <c r="G217" s="5"/>
     </row>
-    <row r="218" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="218" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F218" s="19"/>
       <c r="G218" s="5"/>
     </row>
-    <row r="219" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="219" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F219" s="19"/>
       <c r="G219" s="5"/>
     </row>
-    <row r="220" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="220" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F220" s="19"/>
       <c r="G220" s="5"/>
     </row>
-    <row r="221" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="221" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F221" s="19"/>
       <c r="G221" s="5"/>
     </row>
-    <row r="222" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="222" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F222" s="19"/>
       <c r="G222" s="5"/>
     </row>
-    <row r="223" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="223" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F223" s="19"/>
       <c r="G223" s="5"/>
     </row>
-    <row r="224" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="224" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F224" s="19"/>
       <c r="G224" s="5"/>
     </row>
-    <row r="225" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="225" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F225" s="19"/>
       <c r="G225" s="5"/>
     </row>
-    <row r="226" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="226" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F226" s="19"/>
       <c r="G226" s="5"/>
     </row>
-    <row r="227" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="227" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F227" s="19"/>
       <c r="G227" s="5"/>
     </row>
-    <row r="228" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="228" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F228" s="19"/>
       <c r="G228" s="5"/>
     </row>
-    <row r="229" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="229" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F229" s="19"/>
       <c r="G229" s="5"/>
     </row>
-    <row r="230" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="230" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F230" s="19"/>
       <c r="G230" s="5"/>
     </row>
-    <row r="231" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="231" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F231" s="19"/>
       <c r="G231" s="5"/>
     </row>
-    <row r="232" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="232" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F232" s="19"/>
       <c r="G232" s="5"/>
     </row>
-    <row r="233" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="233" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F233" s="19"/>
       <c r="G233" s="5"/>
     </row>
-    <row r="234" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="234" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F234" s="19"/>
       <c r="G234" s="5"/>
     </row>
-    <row r="235" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="235" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F235" s="19"/>
       <c r="G235" s="5"/>
     </row>
-    <row r="236" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="236" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F236" s="19"/>
       <c r="G236" s="5"/>
     </row>
-    <row r="237" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="237" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F237" s="19"/>
       <c r="G237" s="5"/>
     </row>
-    <row r="238" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="238" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F238" s="19"/>
       <c r="G238" s="5"/>
     </row>
-    <row r="239" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="239" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F239" s="19"/>
       <c r="G239" s="5"/>
     </row>
-    <row r="240" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="240" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F240" s="19"/>
       <c r="G240" s="5"/>
     </row>
-    <row r="241" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="241" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F241" s="19"/>
       <c r="G241" s="5"/>
     </row>
-    <row r="242" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="242" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F242" s="19"/>
       <c r="G242" s="5"/>
     </row>
-    <row r="243" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="243" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F243" s="19"/>
       <c r="G243" s="5"/>
     </row>
-    <row r="244" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="244" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F244" s="19"/>
       <c r="G244" s="5"/>
     </row>
-    <row r="245" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="245" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F245" s="19"/>
       <c r="G245" s="5"/>
     </row>
-    <row r="246" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="246" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F246" s="19"/>
       <c r="G246" s="5"/>
     </row>
-    <row r="247" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="247" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F247" s="19"/>
       <c r="G247" s="5"/>
     </row>
-    <row r="248" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="248" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F248" s="19"/>
       <c r="G248" s="5"/>
     </row>
-    <row r="249" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="249" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F249" s="19"/>
       <c r="G249" s="5"/>
     </row>
-    <row r="250" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="250" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F250" s="19"/>
       <c r="G250" s="5"/>
     </row>
-    <row r="251" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="251" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F251" s="19"/>
       <c r="G251" s="5"/>
     </row>
-    <row r="252" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="252" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F252" s="19"/>
       <c r="G252" s="5"/>
     </row>
-    <row r="253" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="253" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F253" s="19"/>
       <c r="G253" s="5"/>
     </row>
-    <row r="254" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="254" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F254" s="19"/>
       <c r="G254" s="5"/>
     </row>
-    <row r="255" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="255" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F255" s="19"/>
       <c r="G255" s="5"/>
     </row>
-    <row r="256" spans="6:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="256" spans="6:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F256" s="20"/>
       <c r="G256" s="5"/>
     </row>
@@ -2446,15 +2446,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100456CA6835902874B8BE082FCF13655C6" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="75e32df1ccc6cbc2725b15495093f8d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57ea0966535b2bffddf5ddee7861ef65">
     <xsd:element name="properties">
@@ -2568,6 +2559,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2575,14 +2575,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{231BEEE7-30B5-4349-9BCD-5E5310903C59}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0EAA49-81C5-49D2-8213-D1127B60D960}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2594,6 +2586,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{231BEEE7-30B5-4349-9BCD-5E5310903C59}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>